<commit_message>
output, #278: Add dice_report sheet.
</commit_message>
<xml_diff>
--- a/co2mpas/co2mpas_output_template.xlsx
+++ b/co2mpas/co2mpas_output_template.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26101"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16200"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="16200"/>
   </bookViews>
   <sheets>
     <sheet name="output_report" sheetId="22" r:id="rId1"/>
+    <sheet name="dice_report" sheetId="23" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>CO2MPAS version</t>
   </si>
@@ -198,6 +194,24 @@
   </si>
   <si>
     <t>CO2 emission phase Extra-High</t>
+  </si>
+  <si>
+    <t>CO2MPAS error - vehicle H (%)</t>
+  </si>
+  <si>
+    <t>CO2MPAS error - vehicle L (%)</t>
+  </si>
+  <si>
+    <t>Fuel Type</t>
+  </si>
+  <si>
+    <t>Engine Capacity (cc)</t>
+  </si>
+  <si>
+    <t>Gearbox type</t>
+  </si>
+  <si>
+    <t>Turbo engine</t>
   </si>
 </sst>
 </file>
@@ -491,7 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -594,6 +608,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -899,16 +925,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="39.83203125" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -1020,7 +1046,7 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
     </row>
-    <row r="6" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
@@ -1066,7 +1092,7 @@
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
     </row>
-    <row r="8" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="17.100000000000001" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
@@ -1124,7 +1150,7 @@
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
     </row>
-    <row r="10" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>11</v>
       </c>
@@ -1174,7 +1200,7 @@
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
     </row>
-    <row r="12" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="19"/>
       <c r="C12" s="3"/>
@@ -1276,7 +1302,7 @@
       <c r="P15" s="8"/>
       <c r="Q15" s="8"/>
     </row>
-    <row r="16" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>17</v>
       </c>
@@ -1966,4 +1992,108 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="e">
+        <f>IF([0]!_info_CO2MPAS_version_Value&lt;&gt;"",[0]!_info_CO2MPAS_version_Value,"")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="e">
+        <f>IF([0]!_info_Simulation_started_Value&lt;&gt;"",[0]!_info_Simulation_started_Value,"")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="40" t="e">
+        <f>IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio-1)*100,"")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="40" t="e">
+        <f>IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio-1)*100,"")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="38" t="e">
+        <f>IF([0]!_results_nedc_h_prediction_output_vehicle_fuel_type__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_fuel_type__,"")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="37" t="e">
+        <f>IF([0]!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_,"")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="37" t="e">
+        <f>IF([0]!_results_nedc_h_prediction_output_vehicle_gear_box_type__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_gear_box_type__,"")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="39" t="e">
+        <f>IF([0]!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__,"")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
output, #278: Update co2mpas_output_template margins.
</commit_message>
<xml_diff>
--- a/co2mpas/co2mpas_output_template.xlsx
+++ b/co2mpas/co2mpas_output_template.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="16200"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16200"/>
   </bookViews>
   <sheets>
     <sheet name="output_report" sheetId="22" r:id="rId1"/>
     <sheet name="dice_report" sheetId="24" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -235,7 +240,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +312,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -530,7 +541,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -540,7 +551,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -809,7 +820,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -844,7 +855,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1055,20 +1066,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="0.42578125" style="4" hidden="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="4" hidden="1"/>
+    <col min="1" max="1" width="35.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0.5" style="4" hidden="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="4" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1092,7 +1103,7 @@
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
     </row>
-    <row r="2" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1127,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1140,7 +1151,7 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -1164,7 +1175,7 @@
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
     </row>
-    <row r="5" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="2"/>
@@ -1183,7 +1194,7 @@
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
     </row>
-    <row r="6" spans="1:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
@@ -1202,7 +1213,7 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7" spans="1:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -1229,7 +1240,7 @@
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
     </row>
-    <row r="8" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -1258,7 +1269,7 @@
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
     </row>
-    <row r="9" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>9</v>
       </c>
@@ -1287,7 +1298,7 @@
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
     </row>
-    <row r="10" spans="1:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>38</v>
       </c>
@@ -1316,7 +1327,7 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
     </row>
-    <row r="11" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>11</v>
       </c>
@@ -1337,7 +1348,7 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
     </row>
-    <row r="12" spans="1:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="23"/>
       <c r="C12" s="2"/>
@@ -1356,7 +1367,7 @@
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
     </row>
-    <row r="13" spans="1:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -1381,7 +1392,7 @@
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
     </row>
-    <row r="14" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>13</v>
       </c>
@@ -1410,7 +1421,7 @@
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
     </row>
-    <row r="15" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>14</v>
       </c>
@@ -1439,7 +1450,7 @@
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
     </row>
-    <row r="16" spans="1:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>15</v>
       </c>
@@ -1468,7 +1479,7 @@
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
     </row>
-    <row r="17" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="23"/>
       <c r="C17" s="2"/>
@@ -1487,7 +1498,7 @@
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
     </row>
-    <row r="18" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="23"/>
       <c r="C18" s="2"/>
@@ -1506,7 +1517,7 @@
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
     </row>
-    <row r="19" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="29" t="s">
         <v>16</v>
       </c>
@@ -1531,7 +1542,7 @@
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
     </row>
-    <row r="20" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
         <v>17</v>
       </c>
@@ -1560,7 +1571,7 @@
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
     </row>
-    <row r="21" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
         <v>19</v>
       </c>
@@ -1589,7 +1600,7 @@
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
     </row>
-    <row r="22" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="31" t="s">
         <v>21</v>
       </c>
@@ -1618,7 +1629,7 @@
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
     </row>
-    <row r="23" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="30" t="s">
         <v>22</v>
       </c>
@@ -1647,7 +1658,7 @@
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
     </row>
-    <row r="24" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="29" t="s">
         <v>24</v>
       </c>
@@ -1672,7 +1683,7 @@
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
     </row>
-    <row r="25" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="30" t="s">
         <v>17</v>
       </c>
@@ -1701,7 +1712,7 @@
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
     </row>
-    <row r="26" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="31" t="s">
         <v>19</v>
       </c>
@@ -1730,7 +1741,7 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
     </row>
-    <row r="27" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
         <v>21</v>
       </c>
@@ -1759,7 +1770,7 @@
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
     </row>
-    <row r="28" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="30" t="s">
         <v>25</v>
       </c>
@@ -1788,7 +1799,7 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
     </row>
-    <row r="29" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="30" t="s">
         <v>26</v>
       </c>
@@ -1817,7 +1828,7 @@
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
     </row>
-    <row r="30" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="30" t="s">
         <v>27</v>
       </c>
@@ -1846,7 +1857,7 @@
       <c r="P30" s="6"/>
       <c r="Q30" s="6"/>
     </row>
-    <row r="31" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="30" t="s">
         <v>28</v>
       </c>
@@ -1875,7 +1886,7 @@
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
     </row>
-    <row r="32" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="30" t="s">
         <v>29</v>
       </c>
@@ -1904,7 +1915,7 @@
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
     </row>
-    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1923,7 +1934,7 @@
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
     </row>
-    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1942,7 +1953,7 @@
       <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
     </row>
-    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1961,7 +1972,7 @@
       <c r="P35" s="6"/>
       <c r="Q35" s="6"/>
     </row>
-    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1980,7 +1991,7 @@
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
     </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -1999,7 +2010,7 @@
       <c r="P37" s="6"/>
       <c r="Q37" s="6"/>
     </row>
-    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -2018,7 +2029,7 @@
       <c r="P38" s="6"/>
       <c r="Q38" s="6"/>
     </row>
-    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -2037,7 +2048,7 @@
       <c r="P39" s="6"/>
       <c r="Q39" s="6"/>
     </row>
-    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -2056,7 +2067,7 @@
       <c r="P40" s="6"/>
       <c r="Q40" s="6"/>
     </row>
-    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -2075,7 +2086,7 @@
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
     </row>
-    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -2094,7 +2105,7 @@
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
     </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -2115,6 +2126,7 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="B10:C10">
     <cfRule type="colorScale" priority="5">
       <colorScale>
@@ -2135,11 +2147,16 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;CCO2MPAS SUMMARY OUTPUT REPORT</oddHeader>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2147,20 +2164,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFC10"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" style="40" customWidth="1"/>
     <col min="2" max="2" width="40" style="41" customWidth="1"/>
-    <col min="3" max="3" width="0.140625" style="35" customWidth="1"/>
-    <col min="4" max="16383" width="9.140625" style="35" hidden="1"/>
-    <col min="16384" max="16384" width="0.5703125" style="35" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="0.1640625" style="35" customWidth="1"/>
+    <col min="4" max="16383" width="9.1640625" style="35" hidden="1"/>
+    <col min="16384" max="16384" width="0.5" style="35" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2169,7 +2186,7 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2178,7 +2195,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2187,7 +2204,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -2196,7 +2213,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -2205,7 +2222,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -2214,7 +2231,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -2223,7 +2240,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -2232,7 +2249,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -2241,7 +2258,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
@@ -2252,6 +2269,7 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="B5:B6">
     <cfRule type="colorScale" priority="4">
       <colorScale>
@@ -2272,10 +2290,15 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;CCO2MPAS DICE REPORT</oddHeader>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
output, #278: Update dice report adding models scores.
</commit_message>
<xml_diff>
--- a/co2mpas/co2mpas_output_template.xlsx
+++ b/co2mpas/co2mpas_output_template.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="37395" windowHeight="15480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15480"/>
   </bookViews>
   <sheets>
     <sheet name="output_report" sheetId="4" r:id="rId1"/>
-    <sheet name="dice_report" sheetId="5" r:id="rId2"/>
+    <sheet name="dice_report" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
   <si>
     <t>TA Certificate Number</t>
   </si>
@@ -204,22 +217,79 @@
     <t>CO2 emission phase Extra-High</t>
   </si>
   <si>
-    <t>CO2MPAS error - vehicle H (%)</t>
-  </si>
-  <si>
-    <t>CO2MPAS error - vehicle L (%)</t>
-  </si>
-  <si>
     <t>Fuel Type</t>
   </si>
   <si>
-    <t>Engine Capacity (cc)</t>
-  </si>
-  <si>
     <t>Gearbox type</t>
   </si>
   <si>
     <t>Turbo engine</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Engine Capacity</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>alternator_model</t>
+  </si>
+  <si>
+    <t>at_model</t>
+  </si>
+  <si>
+    <t>clutch_torque_converter_model</t>
+  </si>
+  <si>
+    <t>co2_params</t>
+  </si>
+  <si>
+    <t>engine_cold_start_speed_model</t>
+  </si>
+  <si>
+    <t>engine_coolant_temperature_model</t>
+  </si>
+  <si>
+    <t>engine_speed_model</t>
+  </si>
+  <si>
+    <t>start_stop_model</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <r>
+      <t>CO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>g/s</t>
+    </r>
+  </si>
+  <si>
+    <t>°C</t>
   </si>
 </sst>
 </file>
@@ -230,7 +300,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,8 +366,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -341,7 +425,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -524,21 +608,74 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color auto="1"/>
       </left>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -546,7 +683,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -688,33 +825,40 @@
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="5" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -740,14 +884,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -804,12 +948,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -839,12 +983,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1050,20 +1194,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" view="pageLayout" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="0.42578125" style="5" hidden="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="5" hidden="1"/>
+    <col min="1" max="1" width="35.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0.5" style="5" hidden="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1231,7 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1111,7 +1255,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1135,7 +1279,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1159,7 +1303,7 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
@@ -1178,7 +1322,7 @@
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
     </row>
-    <row r="6" spans="1:17" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
@@ -1197,7 +1341,7 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
     </row>
-    <row r="7" spans="1:17" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
@@ -1224,7 +1368,7 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
     </row>
-    <row r="8" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>8</v>
       </c>
@@ -1253,7 +1397,7 @@
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
     </row>
-    <row r="9" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>10</v>
       </c>
@@ -1282,7 +1426,7 @@
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
     </row>
-    <row r="10" spans="1:17" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>11</v>
       </c>
@@ -1311,7 +1455,7 @@
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
     </row>
-    <row r="11" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>13</v>
       </c>
@@ -1332,7 +1476,7 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
     </row>
-    <row r="12" spans="1:17" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="24"/>
       <c r="C12" s="3"/>
@@ -1351,7 +1495,7 @@
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
     </row>
-    <row r="13" spans="1:17" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
@@ -1376,7 +1520,7 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
     </row>
-    <row r="14" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
@@ -1405,7 +1549,7 @@
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
     </row>
-    <row r="15" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>16</v>
       </c>
@@ -1434,7 +1578,7 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="1:17" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>17</v>
       </c>
@@ -1463,7 +1607,7 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
     </row>
-    <row r="17" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="24"/>
       <c r="C17" s="3"/>
@@ -1482,7 +1626,7 @@
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
     </row>
-    <row r="18" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="24"/>
       <c r="C18" s="3"/>
@@ -1501,7 +1645,7 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
         <v>18</v>
       </c>
@@ -1526,7 +1670,7 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
         <v>19</v>
       </c>
@@ -1555,7 +1699,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>21</v>
       </c>
@@ -1584,7 +1728,7 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
     </row>
-    <row r="22" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>23</v>
       </c>
@@ -1613,7 +1757,7 @@
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
     </row>
-    <row r="23" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
         <v>25</v>
       </c>
@@ -1642,7 +1786,7 @@
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
     </row>
-    <row r="24" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
         <v>27</v>
       </c>
@@ -1667,7 +1811,7 @@
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
     </row>
-    <row r="25" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="31" t="s">
         <v>19</v>
       </c>
@@ -1696,7 +1840,7 @@
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
     </row>
-    <row r="26" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
         <v>21</v>
       </c>
@@ -1725,7 +1869,7 @@
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
     </row>
-    <row r="27" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
         <v>23</v>
       </c>
@@ -1754,7 +1898,7 @@
       <c r="P27" s="7"/>
       <c r="Q27" s="7"/>
     </row>
-    <row r="28" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="31" t="s">
         <v>28</v>
       </c>
@@ -1783,7 +1927,7 @@
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
     </row>
-    <row r="29" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="31" t="s">
         <v>29</v>
       </c>
@@ -1812,7 +1956,7 @@
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
     </row>
-    <row r="30" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="31" t="s">
         <v>30</v>
       </c>
@@ -1841,7 +1985,7 @@
       <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
     </row>
-    <row r="31" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="31" t="s">
         <v>31</v>
       </c>
@@ -1870,7 +2014,7 @@
       <c r="P31" s="7"/>
       <c r="Q31" s="7"/>
     </row>
-    <row r="32" spans="1:17" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="31" t="s">
         <v>32</v>
       </c>
@@ -1899,7 +2043,7 @@
       <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
     </row>
-    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1918,7 +2062,7 @@
       <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
     </row>
-    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1937,7 +2081,7 @@
       <c r="P34" s="7"/>
       <c r="Q34" s="7"/>
     </row>
-    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1956,7 +2100,7 @@
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
     </row>
-    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1975,7 +2119,7 @@
       <c r="P36" s="7"/>
       <c r="Q36" s="7"/>
     </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1994,7 +2138,7 @@
       <c r="P37" s="7"/>
       <c r="Q37" s="7"/>
     </row>
-    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -2013,7 +2157,7 @@
       <c r="P38" s="7"/>
       <c r="Q38" s="7"/>
     </row>
-    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -2032,7 +2176,7 @@
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
     </row>
-    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -2051,7 +2195,7 @@
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
     </row>
-    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -2070,7 +2214,7 @@
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
     </row>
-    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -2089,7 +2233,7 @@
       <c r="P42" s="7"/>
       <c r="Q42" s="7"/>
     </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -2110,6 +2254,7 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B10:C10">
     <cfRule type="colorScale" priority="3">
       <colorScale>
@@ -2123,10 +2268,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$B$4="False"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$B$4="True"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2135,120 +2280,607 @@
   <headerFooter>
     <oddHeader>&amp;CCO2MPAS SUMMARY OUTPUT REPORT</oddHeader>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFC10"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" view="pageLayout" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39" style="42" customWidth="1"/>
-    <col min="2" max="2" width="40" style="43" customWidth="1"/>
-    <col min="3" max="3" width="0.140625" style="37" customWidth="1"/>
-    <col min="4" max="16383" width="9.140625" style="37" hidden="1"/>
-    <col min="16384" max="16384" width="0.42578125" style="37" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="36" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0.5" style="36" hidden="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="36" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="str">
-        <f>IFERROR(IF([0]!_info_ta_certificate_number_Value&lt;&gt;"",[0]!_info_ta_certificate_number_Value,""),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="str">
+        <f>IFERROR(IF([0]!_info_ta_certificate_number_Value&lt;&gt;"",[0]!_info_ta_certificate_number_Value,""), "")</f>
+        <v/>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36" t="str">
-        <f>IFERROR(IF([0]!_info_CO2MPAS_version_Value&lt;&gt;"",[0]!_info_CO2MPAS_version_Value,""),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="str">
+        <f>IFERROR(IF([0]!_info_CO2MPAS_version_Value&lt;&gt;"",[0]!_info_CO2MPAS_version_Value,""), "")</f>
+        <v/>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="str">
+      <c r="B3" s="2" t="str">
         <f>IFERROR(IF([0]!_info_Simulation_started_Value&lt;&gt;"",[0]!_info_Simulation_started_Value,""),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="38" t="str">
+      <c r="B4" s="6" t="str">
         <f>IFERROR(IF([0]!_info_type_approval_mode_Value&lt;&gt;"",[0]!_info_type_approval_mode_Value,""),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+    </row>
+    <row r="5" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+    </row>
+    <row r="6" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+    </row>
+    <row r="7" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="37"/>
+      <c r="B7" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+    </row>
+    <row r="8" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="39" t="str">
+      <c r="B8" s="41" t="str">
+        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_fuel_type__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_fuel_type__,""),"")</f>
+        <v/>
+      </c>
+      <c r="C8" s="42" t="str">
+        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_fuel_type__&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_fuel_type__,""),"")</f>
+        <v/>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+    </row>
+    <row r="9" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="26" t="str">
+        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_,""),"")</f>
+        <v/>
+      </c>
+      <c r="C9" s="27" t="str">
+        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_,""),"")</f>
+        <v/>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+    </row>
+    <row r="10" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="26" t="str">
+        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_gear_box_type__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_gear_box_type__,""),"")</f>
+        <v/>
+      </c>
+      <c r="C10" s="27" t="str">
+        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_gear_box_type__&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_gear_box_type__,""),"")</f>
+        <v/>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+    </row>
+    <row r="11" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="26" t="str">
+        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__,""),"")</f>
+        <v/>
+      </c>
+      <c r="C11" s="27" t="str">
+        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__,""),"")</f>
+        <v/>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+    </row>
+    <row r="12" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="43" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_alternator_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_alternator_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C12" s="44" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_alternator_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_alternator_model_wltp_l_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+    </row>
+    <row r="13" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="43" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_at_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_at_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C13" s="44" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_at_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_at_model_wltp_l_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+    </row>
+    <row r="14" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="43" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_clutch_torque_converter_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_clutch_torque_converter_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C14" s="44" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_clutch_torque_converter_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_clutch_torque_converter_model_wltp_l_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+    </row>
+    <row r="15" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="43" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_co2_params_wltp_h_score&lt;&gt;"",[0]!_score_by_model_co2_params_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C15" s="44" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_co2_params_wltp_l_score&lt;&gt;"",[0]!_score_by_model_co2_params_wltp_l_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+    </row>
+    <row r="16" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="43" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_cold_start_speed_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_cold_start_speed_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C16" s="44" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_cold_start_speed_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_cold_start_speed_model_wltp_l_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+    </row>
+    <row r="17" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="43" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_coolant_temperature_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_coolant_temperature_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C17" s="44" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_coolant_temperature_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_coolant_temperature_model_wltp_l_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+    </row>
+    <row r="18" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="43" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_speed_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_speed_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C18" s="44" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_speed_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_speed_model_wltp_l_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+    </row>
+    <row r="19" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="43" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_start_stop_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_start_stop_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C19" s="44" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_start_stop_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_start_stop_model_wltp_l_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+    </row>
+    <row r="20" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="19" t="str">
         <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio-1)*100,""),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="39" t="str">
+      <c r="C20" s="20" t="str">
         <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio-1)*100,""),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="40" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_fuel_type__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_fuel_type__,""),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="36" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_,""),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="36" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_gear_box_type__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_gear_box_type__,""),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="41" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__,""),"")</f>
-        <v/>
-      </c>
-    </row>
+      <c r="D20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+    </row>
+    <row r="21" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <conditionalFormatting sqref="B5:B6">
-    <cfRule type="colorScale" priority="3">
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="B20:C20">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="num" val="-4"/>
         <cfvo type="num" val="0"/>
@@ -2260,11 +2892,91 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="1" priority="12">
       <formula>$B$4="False"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="0" priority="13">
       <formula>$B$4="True"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:C12">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="60"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:C13">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="num" val="-1"/>
+        <cfvo type="num" val="0"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:C14">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:C15">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:C16">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:C17">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:C18">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="40"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:C19">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="-1"/>
+        <cfvo type="num" val="-0.7"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2272,5 +2984,10 @@
   <headerFooter>
     <oddHeader>&amp;CCO2MPAS DICE REPORT</oddHeader>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
output, #278: Add sub models uuid to the dice report.
</commit_message>
<xml_diff>
--- a/co2mpas/co2mpas_output_template.xlsx
+++ b/co2mpas/co2mpas_output_template.xlsx
@@ -1,34 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15480"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="37395" windowHeight="16755"/>
   </bookViews>
   <sheets>
-    <sheet name="output_report" sheetId="4" r:id="rId1"/>
-    <sheet name="dice_report" sheetId="6" r:id="rId2"/>
+    <sheet name="output_report" sheetId="5" r:id="rId1"/>
+    <sheet name="dice_report" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
   <si>
     <t>TA Certificate Number</t>
   </si>
@@ -40,6 +27,99 @@
   </si>
   <si>
     <t>Type approval mode</t>
+  </si>
+  <si>
+    <t>Vehicle H</t>
+  </si>
+  <si>
+    <t>Vehicle L</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>Fuel Type</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Engine Capacity</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>Gearbox type</t>
+  </si>
+  <si>
+    <t>Turbo engine</t>
+  </si>
+  <si>
+    <t>sub_models_uuid</t>
+  </si>
+  <si>
+    <t>alternator_model score</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>at_model score</t>
+  </si>
+  <si>
+    <t>clutch_torque_converter_model score</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>co2_params score</t>
+  </si>
+  <si>
+    <r>
+      <t>CO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>g/s</t>
+    </r>
+  </si>
+  <si>
+    <t>engine_cold_start_speed_model score</t>
+  </si>
+  <si>
+    <t>engine_coolant_temperature_model score</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>engine_speed_model score</t>
+  </si>
+  <si>
+    <t>start_stop_model score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2MPAS deviation </t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
   <si>
     <r>
@@ -70,15 +150,6 @@
     </r>
   </si>
   <si>
-    <t>Vehicle H</t>
-  </si>
-  <si>
-    <t>Vehicle L</t>
-  </si>
-  <si>
-    <t>units</t>
-  </si>
-  <si>
     <r>
       <t>NEDC CO</t>
     </r>
@@ -113,12 +184,6 @@
     <t xml:space="preserve">NEDC CO2MPAS simulated </t>
   </si>
   <si>
-    <t xml:space="preserve">CO2MPAS deviation </t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
     <t>*Ki factor - corrected</t>
   </si>
   <si>
@@ -216,81 +281,6 @@
   <si>
     <t>CO2 emission phase Extra-High</t>
   </si>
-  <si>
-    <t>Fuel Type</t>
-  </si>
-  <si>
-    <t>Gearbox type</t>
-  </si>
-  <si>
-    <t>Turbo engine</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Engine Capacity</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>alternator_model</t>
-  </si>
-  <si>
-    <t>at_model</t>
-  </si>
-  <si>
-    <t>clutch_torque_converter_model</t>
-  </si>
-  <si>
-    <t>co2_params</t>
-  </si>
-  <si>
-    <t>engine_cold_start_speed_model</t>
-  </si>
-  <si>
-    <t>engine_coolant_temperature_model</t>
-  </si>
-  <si>
-    <t>engine_speed_model</t>
-  </si>
-  <si>
-    <t>start_stop_model</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>RPM</t>
-  </si>
-  <si>
-    <r>
-      <t>CO</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>g/s</t>
-    </r>
-  </si>
-  <si>
-    <t>°C</t>
-  </si>
 </sst>
 </file>
 
@@ -300,7 +290,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,7 +324,7 @@
     </font>
     <font>
       <b/>
-      <vertAlign val="subscript"/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -342,7 +332,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
       <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -359,27 +364,6 @@
     </font>
     <font>
       <vertAlign val="superscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="subscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -458,165 +442,6 @@
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -673,6 +498,165 @@
       <top style="medium">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -683,7 +667,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -713,15 +697,15 @@
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -729,51 +713,131 @@
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -785,19 +849,19 @@
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -823,42 +887,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="5" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -948,12 +976,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -983,12 +1011,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1194,20 +1222,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="35.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="0.5" style="5" hidden="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="5" hidden="1"/>
+    <col min="1" max="1" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0.42578125" style="5" hidden="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="18.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1231,7 +1259,7 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="18.95" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1255,7 +1283,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="18.95" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1279,7 +1307,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="18.95" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1303,7 +1331,7 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="18.95" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
@@ -1322,7 +1350,7 @@
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
     </row>
-    <row r="6" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
@@ -1341,18 +1369,18 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
     </row>
-    <row r="7" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
+      <c r="A7" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="C7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>6</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>7</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -1368,20 +1396,20 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
     </row>
-    <row r="8" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="13" t="str">
+    <row r="8" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A8" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="35" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_target_declared_co2_emission_declared_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_h_prediction_target_declared_co2_emission_declared_value__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="C8" s="14" t="str">
+      <c r="C8" s="36" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_target_declared_co2_emission_declared_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_l_prediction_target_declared_co2_emission_declared_value__CO2g_km_,""),"")</f>
         <v/>
       </c>
       <c r="D8" s="7" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -1397,20 +1425,20 @@
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
     </row>
-    <row r="9" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="18.95" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="16" t="str">
+        <v>31</v>
+      </c>
+      <c r="B9" s="37" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_declared_co2_emission_declared_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_declared_co2_emission_declared_value__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="C9" s="17" t="str">
+      <c r="C9" s="38" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_declared_co2_emission_declared_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_declared_co2_emission_declared_value__CO2g_km_,""),"")</f>
         <v/>
       </c>
       <c r="D9" s="7" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -1426,20 +1454,20 @@
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
     </row>
-    <row r="10" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
       <c r="A10" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="19" t="str">
+        <v>26</v>
+      </c>
+      <c r="B10" s="39" t="str">
         <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio-1)*100,""),"")</f>
         <v/>
       </c>
-      <c r="C10" s="20" t="str">
+      <c r="C10" s="40" t="str">
         <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio-1)*100,""),"")</f>
         <v/>
       </c>
       <c r="D10" s="7" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -1455,12 +1483,12 @@
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
     </row>
-    <row r="11" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
+    <row r="11" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A11" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="42"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1476,15 +1504,15 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
     </row>
-    <row r="12" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
       <c r="A12" s="4"/>
-      <c r="B12" s="24"/>
+      <c r="B12" s="44"/>
       <c r="C12" s="3"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="25"/>
+      <c r="H12" s="45"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
@@ -1495,15 +1523,15 @@
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
     </row>
-    <row r="13" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="9" t="s">
+    <row r="13" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
+      <c r="A13" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="33" t="s">
         <v>5</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>6</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1520,20 +1548,20 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
     </row>
-    <row r="14" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="26" t="str">
+    <row r="14" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A14" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="46" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_co2_emission_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_co2_emission_value__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="C14" s="27" t="str">
+      <c r="C14" s="47" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_co2_emission_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_co2_emission_value__CO2g_km_,""),"")</f>
         <v/>
       </c>
       <c r="D14" s="7" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -1549,20 +1577,20 @@
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
     </row>
-    <row r="15" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="18.95" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="16" t="str">
+        <v>35</v>
+      </c>
+      <c r="B15" s="37" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_co2_emission_UDC__CO2g_km_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_co2_emission_UDC__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="C15" s="17" t="str">
+      <c r="C15" s="38" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_co2_emission_UDC__CO2g_km_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_co2_emission_UDC__CO2g_km_,""),"")</f>
         <v/>
       </c>
       <c r="D15" s="7" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -1578,20 +1606,20 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
       <c r="A16" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="28" t="str">
+        <v>36</v>
+      </c>
+      <c r="B16" s="48" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_co2_emission_EUDC__CO2g_km_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_co2_emission_EUDC__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="C16" s="29" t="str">
+      <c r="C16" s="49" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_co2_emission_EUDC__CO2g_km_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_co2_emission_EUDC__CO2g_km_,""),"")</f>
         <v/>
       </c>
       <c r="D16" s="7" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -1607,9 +1635,9 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
     </row>
-    <row r="17" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="18.95" customHeight="1">
       <c r="A17" s="4"/>
-      <c r="B17" s="24"/>
+      <c r="B17" s="44"/>
       <c r="C17" s="3"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1626,9 +1654,9 @@
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
     </row>
-    <row r="18" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="18.95" customHeight="1">
       <c r="A18" s="4"/>
-      <c r="B18" s="24"/>
+      <c r="B18" s="44"/>
       <c r="C18" s="3"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -1645,15 +1673,15 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="30" t="s">
+    <row r="19" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A19" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="50" t="s">
         <v>5</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>6</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -1670,20 +1698,20 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="16" t="str">
+    <row r="20" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A20" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="37" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_f0__N_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_f0__N_,""),"")</f>
         <v/>
       </c>
-      <c r="C20" s="16" t="str">
+      <c r="C20" s="37" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_f0__N_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_f0__N_,""),"")</f>
         <v/>
       </c>
       <c r="D20" s="7" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -1699,20 +1727,20 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="33" t="str">
+    <row r="21" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A21" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="53" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__,""),"")</f>
         <v/>
       </c>
-      <c r="C21" s="33" t="str">
+      <c r="C21" s="53" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__,""),"")</f>
         <v/>
       </c>
       <c r="D21" s="7" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -1728,20 +1756,20 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
     </row>
-    <row r="22" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="33" t="str">
+    <row r="22" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A22" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="53" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_,""),"")</f>
         <v/>
       </c>
-      <c r="C22" s="33" t="str">
+      <c r="C22" s="53" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_,""),"")</f>
         <v/>
       </c>
       <c r="D22" s="7" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -1757,20 +1785,20 @@
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
     </row>
-    <row r="23" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="34" t="str">
+    <row r="23" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A23" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="54" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_mass__kg_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_mass__kg_,""),"")</f>
         <v/>
       </c>
-      <c r="C23" s="34" t="str">
+      <c r="C23" s="54" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_mass__kg_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_mass__kg_,""),"")</f>
         <v/>
       </c>
-      <c r="D23" s="35" t="s">
-        <v>26</v>
+      <c r="D23" s="55" t="s">
+        <v>45</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -1786,15 +1814,15 @@
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
     </row>
-    <row r="24" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="30" t="s">
+    <row r="24" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A24" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="50" t="s">
         <v>5</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>6</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -1811,20 +1839,20 @@
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
     </row>
-    <row r="25" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="16" t="str">
+    <row r="25" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A25" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="37" t="str">
         <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_vehicle_f0__N_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_vehicle_f0__N_,""),"")</f>
         <v/>
       </c>
-      <c r="C25" s="16" t="str">
+      <c r="C25" s="37" t="str">
         <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_vehicle_f0__N_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_vehicle_f0__N_,""),"")</f>
         <v/>
       </c>
       <c r="D25" s="7" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -1840,20 +1868,20 @@
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
     </row>
-    <row r="26" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="33" t="str">
+    <row r="26" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A26" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="53" t="str">
         <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__&lt;&gt;"",[0]!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__,""),"")</f>
         <v/>
       </c>
-      <c r="C26" s="33" t="str">
+      <c r="C26" s="53" t="str">
         <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__&lt;&gt;"",[0]!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__,""),"")</f>
         <v/>
       </c>
       <c r="D26" s="7" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -1869,20 +1897,20 @@
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
     </row>
-    <row r="27" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="33" t="str">
+    <row r="27" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A27" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="53" t="str">
         <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_,""),"")</f>
         <v/>
       </c>
-      <c r="C27" s="33" t="str">
+      <c r="C27" s="53" t="str">
         <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_,""),"")</f>
         <v/>
       </c>
       <c r="D27" s="7" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -1898,20 +1926,20 @@
       <c r="P27" s="7"/>
       <c r="Q27" s="7"/>
     </row>
-    <row r="28" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="34" t="str">
+    <row r="28" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A28" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="54" t="str">
         <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_vehicle_mass__kg_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_vehicle_mass__kg_,""),"")</f>
         <v/>
       </c>
-      <c r="C28" s="34" t="str">
+      <c r="C28" s="54" t="str">
         <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_vehicle_mass__kg_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_vehicle_mass__kg_,""),"")</f>
         <v/>
       </c>
-      <c r="D28" s="35" t="s">
-        <v>26</v>
+      <c r="D28" s="55" t="s">
+        <v>45</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -1927,20 +1955,20 @@
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
     </row>
-    <row r="29" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="16" t="str">
+    <row r="29" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A29" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="37" t="str">
         <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="C29" s="16" t="str">
+      <c r="C29" s="37" t="str">
         <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="D29" s="35" t="s">
-        <v>9</v>
+      <c r="D29" s="55" t="s">
+        <v>30</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -1956,20 +1984,20 @@
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
     </row>
-    <row r="30" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="31" t="s">
+    <row r="30" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A30" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="37" t="str">
+        <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_,""),"")</f>
+        <v/>
+      </c>
+      <c r="C30" s="37" t="str">
+        <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_,""),"")</f>
+        <v/>
+      </c>
+      <c r="D30" s="55" t="s">
         <v>30</v>
-      </c>
-      <c r="B30" s="16" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C30" s="16" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_,""),"")</f>
-        <v/>
-      </c>
-      <c r="D30" s="35" t="s">
-        <v>9</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -1985,20 +2013,20 @@
       <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
     </row>
-    <row r="31" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="16" t="str">
+    <row r="31" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A31" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="37" t="str">
         <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_,""), "")</f>
         <v/>
       </c>
-      <c r="C31" s="16" t="str">
+      <c r="C31" s="37" t="str">
         <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="D31" s="35" t="s">
-        <v>9</v>
+      <c r="D31" s="55" t="s">
+        <v>30</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -2014,20 +2042,20 @@
       <c r="P31" s="7"/>
       <c r="Q31" s="7"/>
     </row>
-    <row r="32" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="16" t="str">
+    <row r="32" spans="1:17" ht="18.95" customHeight="1">
+      <c r="A32" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="37" t="str">
         <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="C32" s="16" t="str">
+      <c r="C32" s="37" t="str">
         <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="D32" s="35" t="s">
-        <v>9</v>
+      <c r="D32" s="55" t="s">
+        <v>30</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -2043,7 +2071,7 @@
       <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
     </row>
-    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" hidden="1">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2062,7 +2090,7 @@
       <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
     </row>
-    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" hidden="1">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2081,7 +2109,7 @@
       <c r="P34" s="7"/>
       <c r="Q34" s="7"/>
     </row>
-    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" hidden="1">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -2100,7 +2128,7 @@
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
     </row>
-    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" hidden="1">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -2119,7 +2147,7 @@
       <c r="P36" s="7"/>
       <c r="Q36" s="7"/>
     </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" hidden="1">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -2138,7 +2166,7 @@
       <c r="P37" s="7"/>
       <c r="Q37" s="7"/>
     </row>
-    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" hidden="1">
       <c r="A38" s="3"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -2157,7 +2185,7 @@
       <c r="P38" s="7"/>
       <c r="Q38" s="7"/>
     </row>
-    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" hidden="1">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -2176,7 +2204,7 @@
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
     </row>
-    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" hidden="1">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -2195,7 +2223,7 @@
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
     </row>
-    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" hidden="1">
       <c r="A41" s="3"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -2214,7 +2242,7 @@
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
     </row>
-    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" hidden="1">
       <c r="A42" s="3"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -2233,7 +2261,7 @@
       <c r="P42" s="7"/>
       <c r="Q42" s="7"/>
     </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" hidden="1">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -2254,7 +2282,6 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B10:C10">
     <cfRule type="colorScale" priority="3">
       <colorScale>
@@ -2268,10 +2295,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$B$4="False"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$B$4="True"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2280,32 +2307,27 @@
   <headerFooter>
     <oddHeader>&amp;CCO2MPAS SUMMARY OUTPUT REPORT</oddHeader>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q55"/>
+  <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" view="pageLayout" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="35.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.6640625" style="36" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="0.5" style="36" hidden="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="36" hidden="1"/>
+    <col min="1" max="1" width="37.5703125" style="30" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0.42578125" style="30" hidden="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="30" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2329,7 +2351,7 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2353,7 +2375,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2377,7 +2399,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2401,7 +2423,7 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
@@ -2420,7 +2442,7 @@
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
     </row>
-    <row r="6" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
@@ -2439,16 +2461,16 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
     </row>
-    <row r="7" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-      <c r="B7" s="38" t="s">
+    <row r="7" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="D7" s="11" t="s">
         <v>6</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>7</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -2464,20 +2486,20 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
     </row>
-    <row r="8" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="41" t="str">
+    <row r="8" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_fuel_type__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_fuel_type__,""),"")</f>
         <v/>
       </c>
-      <c r="C8" s="42" t="str">
+      <c r="C8" s="14" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_fuel_type__&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_fuel_type__,""),"")</f>
         <v/>
       </c>
       <c r="D8" s="7" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -2493,20 +2515,20 @@
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
     </row>
-    <row r="9" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="26" t="str">
+    <row r="9" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="16" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_,""),"")</f>
         <v/>
       </c>
-      <c r="C9" s="27" t="str">
+      <c r="C9" s="17" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_,""),"")</f>
         <v/>
       </c>
       <c r="D9" s="7" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -2522,20 +2544,20 @@
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
     </row>
-    <row r="10" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="26" t="str">
+    <row r="10" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="16" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_gear_box_type__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_gear_box_type__,""),"")</f>
         <v/>
       </c>
-      <c r="C10" s="27" t="str">
+      <c r="C10" s="17" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_gear_box_type__&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_gear_box_type__,""),"")</f>
         <v/>
       </c>
       <c r="D10" s="7" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -2551,20 +2573,20 @@
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
     </row>
-    <row r="11" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="26" t="str">
+    <row r="11" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
+      <c r="A11" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="19" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__,""),"")</f>
         <v/>
       </c>
-      <c r="C11" s="27" t="str">
+      <c r="C11" s="20" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__,""),"")</f>
         <v/>
       </c>
       <c r="D11" s="7" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -2580,20 +2602,20 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
     </row>
-    <row r="12" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A12" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="43" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_alternator_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_alternator_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C12" s="44" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_alternator_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_alternator_model_wltp_l_score,""),"")</f>
+        <v>13</v>
+      </c>
+      <c r="B12" s="21" t="str">
+        <f>IFERROR(IF([0]!_models_uuid_nedc_h_uuid&lt;&gt;"",[0]!_models_uuid_nedc_h_uuid,""),"")</f>
+        <v/>
+      </c>
+      <c r="C12" s="22" t="str">
+        <f>IFERROR(IF([0]!_models_uuid_nedc_l_uuid&lt;&gt;"",[0]!_models_uuid_nedc_l_uuid,""),"")</f>
         <v/>
       </c>
       <c r="D12" s="7" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -2609,20 +2631,20 @@
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
     </row>
-    <row r="13" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="43" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_at_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_at_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C13" s="44" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_at_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_at_model_wltp_l_score,""),"")</f>
+    <row r="13" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A13" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="23" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_alternator_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_alternator_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C13" s="24" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_alternator_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_alternator_model_wltp_l_score,""),"")</f>
         <v/>
       </c>
       <c r="D13" s="7" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -2638,20 +2660,20 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
     </row>
-    <row r="14" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="43" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_clutch_torque_converter_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_clutch_torque_converter_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C14" s="44" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_clutch_torque_converter_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_clutch_torque_converter_model_wltp_l_score,""),"")</f>
+    <row r="14" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A14" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="23" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_at_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_at_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C14" s="24" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_at_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_at_model_wltp_l_score,""),"")</f>
         <v/>
       </c>
       <c r="D14" s="7" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -2667,20 +2689,20 @@
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
     </row>
-    <row r="15" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="43" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_co2_params_wltp_h_score&lt;&gt;"",[0]!_score_by_model_co2_params_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C15" s="44" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_co2_params_wltp_l_score&lt;&gt;"",[0]!_score_by_model_co2_params_wltp_l_score,""),"")</f>
+    <row r="15" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A15" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="23" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_clutch_torque_converter_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_clutch_torque_converter_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C15" s="24" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_clutch_torque_converter_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_clutch_torque_converter_model_wltp_l_score,""),"")</f>
         <v/>
       </c>
       <c r="D15" s="7" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -2696,20 +2718,20 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="43" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_cold_start_speed_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_cold_start_speed_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C16" s="44" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_cold_start_speed_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_cold_start_speed_model_wltp_l_score,""),"")</f>
+    <row r="16" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="23" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_co2_params_wltp_h_score&lt;&gt;"",[0]!_score_by_model_co2_params_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C16" s="24" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_co2_params_wltp_l_score&lt;&gt;"",[0]!_score_by_model_co2_params_wltp_l_score,""),"")</f>
         <v/>
       </c>
       <c r="D16" s="7" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -2725,20 +2747,20 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
     </row>
-    <row r="17" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="43" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_coolant_temperature_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_coolant_temperature_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C17" s="44" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_coolant_temperature_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_coolant_temperature_model_wltp_l_score,""),"")</f>
+    <row r="17" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A17" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="23" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_cold_start_speed_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_cold_start_speed_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C17" s="24" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_cold_start_speed_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_cold_start_speed_model_wltp_l_score,""),"")</f>
         <v/>
       </c>
       <c r="D17" s="7" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -2754,20 +2776,20 @@
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
     </row>
-    <row r="18" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="43" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_speed_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_speed_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C18" s="44" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_speed_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_speed_model_wltp_l_score,""),"")</f>
+    <row r="18" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+      <c r="A18" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="23" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_coolant_temperature_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_coolant_temperature_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C18" s="24" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_coolant_temperature_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_coolant_temperature_model_wltp_l_score,""),"")</f>
         <v/>
       </c>
       <c r="D18" s="7" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -2783,20 +2805,20 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A19" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="43" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_start_stop_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_start_stop_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C19" s="44" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_start_stop_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_start_stop_model_wltp_l_score,""),"")</f>
+        <v>24</v>
+      </c>
+      <c r="B19" s="23" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_speed_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_speed_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C19" s="24" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_speed_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_speed_model_wltp_l_score,""),"")</f>
         <v/>
       </c>
       <c r="D19" s="7" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -2812,20 +2834,20 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
       <c r="A20" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="19" t="str">
-        <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio-1)*100,""),"")</f>
-        <v/>
-      </c>
-      <c r="C20" s="20" t="str">
-        <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio-1)*100,""),"")</f>
+        <v>25</v>
+      </c>
+      <c r="B20" s="25" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_start_stop_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_start_stop_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C20" s="26" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_start_stop_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_start_stop_model_wltp_l_score,""),"")</f>
         <v/>
       </c>
       <c r="D20" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -2841,46 +2863,88 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
+      <c r="A21" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="28" t="str">
+        <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio-1)*100,""),"")</f>
+        <v/>
+      </c>
+      <c r="C21" s="29" t="str">
+        <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio-1)*100,""),"")</f>
+        <v/>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+    </row>
+    <row r="22" spans="1:17" s="5" customFormat="1" ht="18.95" hidden="1" customHeight="1">
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+    </row>
+    <row r="23" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="24" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="25" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="26" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="27" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="28" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="29" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="30" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="31" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="32" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="33" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="34" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="35" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="36" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="37" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="38" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="39" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="40" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="41" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="42" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="43" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="44" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="45" ht="15" hidden="1" customHeight="1"/>
+    <row r="46" ht="15" hidden="1" customHeight="1"/>
+    <row r="47" ht="15" hidden="1" customHeight="1"/>
+    <row r="48" ht="15" hidden="1" customHeight="1"/>
+    <row r="49" ht="15" hidden="1" customHeight="1"/>
+    <row r="50" ht="15" hidden="1" customHeight="1"/>
+    <row r="51" ht="15" hidden="1" customHeight="1"/>
+    <row r="52" ht="15" hidden="1" customHeight="1"/>
+    <row r="53" ht="15" hidden="1" customHeight="1"/>
+    <row r="54" ht="15" hidden="1" customHeight="1"/>
+    <row r="55" ht="15" hidden="1" customHeight="1"/>
+    <row r="56" ht="15" hidden="1" customHeight="1"/>
+    <row r="57" ht="15" hidden="1" customHeight="1"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="B20:C20">
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="B21:C21">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="num" val="-4"/>
         <cfvo type="num" val="0"/>
@@ -2892,15 +2956,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="1" priority="12">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>$B$4="False"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="13">
+    <cfRule type="expression" dxfId="2" priority="10">
       <formula>$B$4="True"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:C12">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="B13:C13">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -2909,8 +2973,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:C13">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="B14:C14">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="0"/>
@@ -2919,7 +2983,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:C14">
+  <conditionalFormatting sqref="B15:C15">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2929,7 +2993,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:C15">
+  <conditionalFormatting sqref="B16:C16">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2939,7 +3003,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:C16">
+  <conditionalFormatting sqref="B17:C17">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2949,7 +3013,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:C17">
+  <conditionalFormatting sqref="B18:C18">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2959,7 +3023,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:C18">
+  <conditionalFormatting sqref="B19:C19">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2969,7 +3033,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:C19">
+  <conditionalFormatting sqref="B20:C20">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="-1"/>
@@ -2984,10 +3048,5 @@
   <headerFooter>
     <oddHeader>&amp;CCO2MPAS DICE REPORT</oddHeader>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
output, #306, #278 : Update output template with `ta_certificate_number` --> `vehicle_family_id` + remove uuid.
</commit_message>
<xml_diff>
--- a/co2mpas/co2mpas_output_template.xlsx
+++ b/co2mpas/co2mpas_output_template.xlsx
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
-  <si>
-    <t>TA Certificate Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
   <si>
     <t>CO2MPAS version</t>
   </si>
@@ -54,9 +51,6 @@
   </si>
   <si>
     <t>Turbo engine</t>
-  </si>
-  <si>
-    <t>sub_models_uuid</t>
   </si>
   <si>
     <t>alternator_model score</t>
@@ -280,6 +274,9 @@
   </si>
   <si>
     <t>CO2 emission phase Extra-High</t>
+  </si>
+  <si>
+    <t>Vehicle Family ID</t>
   </si>
 </sst>
 </file>
@@ -667,7 +664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -747,14 +744,6 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1237,10 +1226,10 @@
   <sheetData>
     <row r="1" spans="1:17" ht="18.95" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="str">
-        <f>IFERROR(IF([0]!_info_ta_certificate_number_Value&lt;&gt;"",[0]!_info_ta_certificate_number_Value,""), "")</f>
+        <f>IFERROR(IF([0]!_info_vehicle_family_id_Value&lt;&gt;"",[0]!_info_vehicle_family_id_Value,""), "")</f>
         <v/>
       </c>
       <c r="C1" s="3"/>
@@ -1261,7 +1250,7 @@
     </row>
     <row r="2" spans="1:17" ht="18.95" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>IFERROR(IF([0]!_info_CO2MPAS_version_Value&lt;&gt;"",[0]!_info_CO2MPAS_version_Value,""), "")</f>
@@ -1285,7 +1274,7 @@
     </row>
     <row r="3" spans="1:17" ht="18.95" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>IFERROR(IF([0]!_info_Simulation_started_Value&lt;&gt;"",[0]!_info_Simulation_started_Value,""),"")</f>
@@ -1309,7 +1298,7 @@
     </row>
     <row r="4" spans="1:17" ht="18.95" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6" t="str">
         <f>IFERROR(IF([0]!_info_type_approval_mode_Value&lt;&gt;"",[0]!_info_type_approval_mode_Value,""),"")</f>
@@ -1370,17 +1359,17 @@
       <c r="Q6" s="7"/>
     </row>
     <row r="7" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
-      <c r="A7" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="32" t="s">
+      <c r="A7" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="D7" s="11" t="s">
         <v>5</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>6</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -1397,19 +1386,19 @@
       <c r="Q7" s="7"/>
     </row>
     <row r="8" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A8" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="35" t="str">
+      <c r="A8" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="33" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_target_declared_co2_emission_declared_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_h_prediction_target_declared_co2_emission_declared_value__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="C8" s="36" t="str">
+      <c r="C8" s="34" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_target_declared_co2_emission_declared_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_l_prediction_target_declared_co2_emission_declared_value__CO2g_km_,""),"")</f>
         <v/>
       </c>
       <c r="D8" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -1427,18 +1416,18 @@
     </row>
     <row r="9" spans="1:17" ht="18.95" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="37" t="str">
+        <v>29</v>
+      </c>
+      <c r="B9" s="35" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_declared_co2_emission_declared_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_declared_co2_emission_declared_value__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="C9" s="38" t="str">
+      <c r="C9" s="36" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_declared_co2_emission_declared_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_declared_co2_emission_declared_value__CO2g_km_,""),"")</f>
         <v/>
       </c>
       <c r="D9" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -1456,18 +1445,18 @@
     </row>
     <row r="10" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
       <c r="A10" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="39" t="str">
+        <v>24</v>
+      </c>
+      <c r="B10" s="37" t="str">
         <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio-1)*100,""),"")</f>
         <v/>
       </c>
-      <c r="C10" s="40" t="str">
+      <c r="C10" s="38" t="str">
         <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio-1)*100,""),"")</f>
         <v/>
       </c>
       <c r="D10" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -1484,11 +1473,11 @@
       <c r="Q10" s="7"/>
     </row>
     <row r="11" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A11" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="43"/>
+      <c r="A11" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="40"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1506,13 +1495,13 @@
     </row>
     <row r="12" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
       <c r="A12" s="4"/>
-      <c r="B12" s="44"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="3"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="45"/>
+      <c r="H12" s="43"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
@@ -1524,14 +1513,14 @@
       <c r="Q12" s="7"/>
     </row>
     <row r="13" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
-      <c r="A13" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="32" t="s">
+      <c r="A13" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="31" t="s">
         <v>4</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>5</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1549,19 +1538,19 @@
       <c r="Q13" s="7"/>
     </row>
     <row r="14" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A14" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="46" t="str">
+      <c r="A14" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="44" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_co2_emission_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_co2_emission_value__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="C14" s="47" t="str">
+      <c r="C14" s="45" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_co2_emission_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_co2_emission_value__CO2g_km_,""),"")</f>
         <v/>
       </c>
       <c r="D14" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -1579,18 +1568,18 @@
     </row>
     <row r="15" spans="1:17" ht="18.95" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="37" t="str">
+        <v>33</v>
+      </c>
+      <c r="B15" s="35" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_co2_emission_UDC__CO2g_km_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_co2_emission_UDC__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="C15" s="38" t="str">
+      <c r="C15" s="36" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_co2_emission_UDC__CO2g_km_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_co2_emission_UDC__CO2g_km_,""),"")</f>
         <v/>
       </c>
       <c r="D15" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -1608,18 +1597,18 @@
     </row>
     <row r="16" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
       <c r="A16" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="48" t="str">
+        <v>34</v>
+      </c>
+      <c r="B16" s="46" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_co2_emission_EUDC__CO2g_km_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_co2_emission_EUDC__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="C16" s="49" t="str">
+      <c r="C16" s="47" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_co2_emission_EUDC__CO2g_km_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_co2_emission_EUDC__CO2g_km_,""),"")</f>
         <v/>
       </c>
       <c r="D16" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -1637,7 +1626,7 @@
     </row>
     <row r="17" spans="1:17" ht="18.95" customHeight="1">
       <c r="A17" s="4"/>
-      <c r="B17" s="44"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="3"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1656,7 +1645,7 @@
     </row>
     <row r="18" spans="1:17" ht="18.95" customHeight="1">
       <c r="A18" s="4"/>
-      <c r="B18" s="44"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="3"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -1674,14 +1663,14 @@
       <c r="Q18" s="7"/>
     </row>
     <row r="19" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A19" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="50" t="s">
+      <c r="A19" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="48" t="s">
         <v>4</v>
-      </c>
-      <c r="C19" s="50" t="s">
-        <v>5</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -1699,19 +1688,19 @@
       <c r="Q19" s="7"/>
     </row>
     <row r="20" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A20" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="37" t="str">
+      <c r="A20" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="35" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_f0__N_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_f0__N_,""),"")</f>
         <v/>
       </c>
-      <c r="C20" s="37" t="str">
+      <c r="C20" s="35" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_f0__N_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_f0__N_,""),"")</f>
         <v/>
       </c>
       <c r="D20" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -1728,19 +1717,19 @@
       <c r="Q20" s="7"/>
     </row>
     <row r="21" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A21" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="53" t="str">
+      <c r="A21" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="51" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__,""),"")</f>
         <v/>
       </c>
-      <c r="C21" s="53" t="str">
+      <c r="C21" s="51" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__,""),"")</f>
         <v/>
       </c>
       <c r="D21" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -1757,19 +1746,19 @@
       <c r="Q21" s="7"/>
     </row>
     <row r="22" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A22" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="53" t="str">
+      <c r="A22" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="51" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_,""),"")</f>
         <v/>
       </c>
-      <c r="C22" s="53" t="str">
+      <c r="C22" s="51" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_,""),"")</f>
         <v/>
       </c>
       <c r="D22" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -1786,19 +1775,19 @@
       <c r="Q22" s="7"/>
     </row>
     <row r="23" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A23" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="54" t="str">
+      <c r="A23" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="52" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_mass__kg_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_mass__kg_,""),"")</f>
         <v/>
       </c>
-      <c r="C23" s="54" t="str">
+      <c r="C23" s="52" t="str">
         <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_mass__kg_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_mass__kg_,""),"")</f>
         <v/>
       </c>
-      <c r="D23" s="55" t="s">
-        <v>45</v>
+      <c r="D23" s="53" t="s">
+        <v>43</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -1815,14 +1804,14 @@
       <c r="Q23" s="7"/>
     </row>
     <row r="24" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A24" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="50" t="s">
+      <c r="A24" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="48" t="s">
         <v>4</v>
-      </c>
-      <c r="C24" s="50" t="s">
-        <v>5</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -1840,19 +1829,19 @@
       <c r="Q24" s="7"/>
     </row>
     <row r="25" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A25" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="37" t="str">
+      <c r="A25" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="35" t="str">
         <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_vehicle_f0__N_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_vehicle_f0__N_,""),"")</f>
         <v/>
       </c>
-      <c r="C25" s="37" t="str">
+      <c r="C25" s="35" t="str">
         <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_vehicle_f0__N_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_vehicle_f0__N_,""),"")</f>
         <v/>
       </c>
       <c r="D25" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -1869,19 +1858,19 @@
       <c r="Q25" s="7"/>
     </row>
     <row r="26" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A26" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="53" t="str">
+      <c r="A26" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="51" t="str">
         <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__&lt;&gt;"",[0]!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__,""),"")</f>
         <v/>
       </c>
-      <c r="C26" s="53" t="str">
+      <c r="C26" s="51" t="str">
         <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__&lt;&gt;"",[0]!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__,""),"")</f>
         <v/>
       </c>
       <c r="D26" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -1898,19 +1887,19 @@
       <c r="Q26" s="7"/>
     </row>
     <row r="27" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A27" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="53" t="str">
+      <c r="A27" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="51" t="str">
         <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_,""),"")</f>
         <v/>
       </c>
-      <c r="C27" s="53" t="str">
+      <c r="C27" s="51" t="str">
         <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_,""),"")</f>
         <v/>
       </c>
       <c r="D27" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -1927,19 +1916,19 @@
       <c r="Q27" s="7"/>
     </row>
     <row r="28" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A28" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="54" t="str">
+      <c r="A28" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="52" t="str">
         <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_vehicle_mass__kg_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_vehicle_mass__kg_,""),"")</f>
         <v/>
       </c>
-      <c r="C28" s="54" t="str">
+      <c r="C28" s="52" t="str">
         <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_vehicle_mass__kg_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_vehicle_mass__kg_,""),"")</f>
         <v/>
       </c>
-      <c r="D28" s="55" t="s">
-        <v>45</v>
+      <c r="D28" s="53" t="s">
+        <v>43</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -1956,19 +1945,19 @@
       <c r="Q28" s="7"/>
     </row>
     <row r="29" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A29" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="37" t="str">
+      <c r="A29" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="35" t="str">
         <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="C29" s="37" t="str">
+      <c r="C29" s="35" t="str">
         <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="D29" s="55" t="s">
-        <v>30</v>
+      <c r="D29" s="53" t="s">
+        <v>28</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -1985,19 +1974,19 @@
       <c r="Q29" s="7"/>
     </row>
     <row r="30" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A30" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="37" t="str">
+      <c r="A30" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="35" t="str">
         <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="C30" s="37" t="str">
+      <c r="C30" s="35" t="str">
         <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="D30" s="55" t="s">
-        <v>30</v>
+      <c r="D30" s="53" t="s">
+        <v>28</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -2014,19 +2003,19 @@
       <c r="Q30" s="7"/>
     </row>
     <row r="31" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A31" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="37" t="str">
+      <c r="A31" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="35" t="str">
         <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_,""), "")</f>
         <v/>
       </c>
-      <c r="C31" s="37" t="str">
+      <c r="C31" s="35" t="str">
         <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="D31" s="55" t="s">
-        <v>30</v>
+      <c r="D31" s="53" t="s">
+        <v>28</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -2043,19 +2032,19 @@
       <c r="Q31" s="7"/>
     </row>
     <row r="32" spans="1:17" ht="18.95" customHeight="1">
-      <c r="A32" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="37" t="str">
+      <c r="A32" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="35" t="str">
         <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="C32" s="37" t="str">
+      <c r="C32" s="35" t="str">
         <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_,""),"")</f>
         <v/>
       </c>
-      <c r="D32" s="55" t="s">
-        <v>30</v>
+      <c r="D32" s="53" t="s">
+        <v>28</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -2281,7 +2270,6 @@
       <c r="Q43" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="B10:C10">
     <cfRule type="colorScale" priority="3">
       <colorScale>
@@ -2295,10 +2283,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$B$4="False"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$B$4="True"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2312,7 +2300,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q57"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -2320,19 +2308,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" style="30" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="0.42578125" style="30" hidden="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="30" hidden="1"/>
+    <col min="1" max="1" width="37.5703125" style="28" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" style="28" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0.42578125" style="28" hidden="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="28" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="str">
-        <f>IFERROR(IF([0]!_info_ta_certificate_number_Value&lt;&gt;"",[0]!_info_ta_certificate_number_Value,""), "")</f>
+        <f>IFERROR(IF([0]!_info_vehicle_family_id_Value&lt;&gt;"",[0]!_info_vehicle_family_id_Value,""), "")</f>
         <v/>
       </c>
       <c r="C1" s="3"/>
@@ -2353,7 +2341,7 @@
     </row>
     <row r="2" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>IFERROR(IF([0]!_info_CO2MPAS_version_Value&lt;&gt;"",[0]!_info_CO2MPAS_version_Value,""), "")</f>
@@ -2377,7 +2365,7 @@
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>IFERROR(IF([0]!_info_Simulation_started_Value&lt;&gt;"",[0]!_info_Simulation_started_Value,""),"")</f>
@@ -2401,7 +2389,7 @@
     </row>
     <row r="4" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6" t="str">
         <f>IFERROR(IF([0]!_info_type_approval_mode_Value&lt;&gt;"",[0]!_info_type_approval_mode_Value,""),"")</f>
@@ -2464,13 +2452,13 @@
     <row r="7" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>5</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>6</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -2488,7 +2476,7 @@
     </row>
     <row r="8" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A8" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="13" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_fuel_type__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_fuel_type__,""),"")</f>
@@ -2499,7 +2487,7 @@
         <v/>
       </c>
       <c r="D8" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -2517,7 +2505,7 @@
     </row>
     <row r="9" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="16" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_,""),"")</f>
@@ -2528,7 +2516,7 @@
         <v/>
       </c>
       <c r="D9" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -2546,7 +2534,7 @@
     </row>
     <row r="10" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="16" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_gear_box_type__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_gear_box_type__,""),"")</f>
@@ -2557,7 +2545,7 @@
         <v/>
       </c>
       <c r="D10" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -2575,7 +2563,7 @@
     </row>
     <row r="11" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
       <c r="A11" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="19" t="str">
         <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__,""),"")</f>
@@ -2586,7 +2574,7 @@
         <v/>
       </c>
       <c r="D11" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -2603,19 +2591,19 @@
       <c r="Q11" s="7"/>
     </row>
     <row r="12" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="21" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_alternator_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_alternator_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C12" s="22" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_alternator_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_alternator_model_wltp_l_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="B12" s="21" t="str">
-        <f>IFERROR(IF([0]!_models_uuid_nedc_h_uuid&lt;&gt;"",[0]!_models_uuid_nedc_h_uuid,""),"")</f>
-        <v/>
-      </c>
-      <c r="C12" s="22" t="str">
-        <f>IFERROR(IF([0]!_models_uuid_nedc_l_uuid&lt;&gt;"",[0]!_models_uuid_nedc_l_uuid,""),"")</f>
-        <v/>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -2635,16 +2623,16 @@
       <c r="A13" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="23" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_alternator_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_alternator_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C13" s="24" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_alternator_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_alternator_model_wltp_l_score,""),"")</f>
+      <c r="B13" s="21" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_at_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_at_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C13" s="22" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_at_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_at_model_wltp_l_score,""),"")</f>
         <v/>
       </c>
       <c r="D13" s="7" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -2662,18 +2650,18 @@
     </row>
     <row r="14" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="21" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_clutch_torque_converter_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_clutch_torque_converter_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C14" s="22" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_clutch_torque_converter_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_clutch_torque_converter_model_wltp_l_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="B14" s="23" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_at_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_at_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C14" s="24" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_at_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_at_model_wltp_l_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -2693,12 +2681,12 @@
       <c r="A15" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="23" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_clutch_torque_converter_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_clutch_torque_converter_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C15" s="24" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_clutch_torque_converter_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_clutch_torque_converter_model_wltp_l_score,""),"")</f>
+      <c r="B15" s="21" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_co2_params_wltp_h_score&lt;&gt;"",[0]!_score_by_model_co2_params_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C15" s="22" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_co2_params_wltp_l_score&lt;&gt;"",[0]!_score_by_model_co2_params_wltp_l_score,""),"")</f>
         <v/>
       </c>
       <c r="D15" s="7" t="s">
@@ -2722,16 +2710,16 @@
       <c r="A16" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="23" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_co2_params_wltp_h_score&lt;&gt;"",[0]!_score_by_model_co2_params_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C16" s="24" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_co2_params_wltp_l_score&lt;&gt;"",[0]!_score_by_model_co2_params_wltp_l_score,""),"")</f>
+      <c r="B16" s="21" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_cold_start_speed_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_cold_start_speed_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C16" s="22" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_cold_start_speed_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_cold_start_speed_model_wltp_l_score,""),"")</f>
         <v/>
       </c>
       <c r="D16" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -2749,18 +2737,18 @@
     </row>
     <row r="17" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
       <c r="A17" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="21" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_coolant_temperature_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_coolant_temperature_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C17" s="22" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_coolant_temperature_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_coolant_temperature_model_wltp_l_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="B17" s="23" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_cold_start_speed_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_cold_start_speed_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C17" s="24" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_cold_start_speed_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_cold_start_speed_model_wltp_l_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -2780,16 +2768,16 @@
       <c r="A18" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="23" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_coolant_temperature_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_coolant_temperature_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C18" s="24" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_coolant_temperature_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_coolant_temperature_model_wltp_l_score,""),"")</f>
+      <c r="B18" s="21" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_speed_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_speed_model_wltp_h_score,""),"")</f>
+        <v/>
+      </c>
+      <c r="C18" s="22" t="str">
+        <f>IFERROR(IF([0]!_score_by_model_engine_speed_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_speed_model_wltp_l_score,""),"")</f>
         <v/>
       </c>
       <c r="D18" s="7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -2805,20 +2793,20 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A19" s="15" t="s">
-        <v>24</v>
+    <row r="19" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
+      <c r="A19" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="B19" s="23" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_speed_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_speed_model_wltp_h_score,""),"")</f>
+        <f>IFERROR(IF([0]!_score_by_model_start_stop_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_start_stop_model_wltp_h_score,""),"")</f>
         <v/>
       </c>
       <c r="C19" s="24" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_speed_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_speed_model_wltp_l_score,""),"")</f>
+        <f>IFERROR(IF([0]!_score_by_model_start_stop_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_start_stop_model_wltp_l_score,""),"")</f>
         <v/>
       </c>
       <c r="D19" s="7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -2835,19 +2823,19 @@
       <c r="Q19" s="7"/>
     </row>
     <row r="20" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="26" t="str">
+        <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio-1)*100,""),"")</f>
+        <v/>
+      </c>
+      <c r="C20" s="27" t="str">
+        <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio-1)*100,""),"")</f>
+        <v/>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="B20" s="25" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_start_stop_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_start_stop_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C20" s="26" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_start_stop_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_start_stop_model_wltp_l_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -2863,21 +2851,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
-      <c r="A21" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="28" t="str">
-        <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio-1)*100,""),"")</f>
-        <v/>
-      </c>
-      <c r="C21" s="29" t="str">
-        <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio-1)*100,""),"")</f>
-        <v/>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>27</v>
-      </c>
+    <row r="21" spans="1:17" s="5" customFormat="1" ht="18.95" hidden="1" customHeight="1">
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -2892,21 +2866,7 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
     </row>
-    <row r="22" spans="1:17" s="5" customFormat="1" ht="18.95" hidden="1" customHeight="1">
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-    </row>
+    <row r="22" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
     <row r="23" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
     <row r="24" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
     <row r="25" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
@@ -2928,7 +2888,7 @@
     <row r="41" ht="18.95" hidden="1" customHeight="1"/>
     <row r="42" ht="18.95" hidden="1" customHeight="1"/>
     <row r="43" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="44" ht="18.95" hidden="1" customHeight="1"/>
+    <row r="44" ht="15" hidden="1" customHeight="1"/>
     <row r="45" ht="15" hidden="1" customHeight="1"/>
     <row r="46" ht="15" hidden="1" customHeight="1"/>
     <row r="47" ht="15" hidden="1" customHeight="1"/>
@@ -2941,9 +2901,9 @@
     <row r="54" ht="15" hidden="1" customHeight="1"/>
     <row r="55" ht="15" hidden="1" customHeight="1"/>
     <row r="56" ht="15" hidden="1" customHeight="1"/>
-    <row r="57" ht="15" hidden="1" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="B21:C21">
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <conditionalFormatting sqref="B20:C20">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="num" val="-4"/>
@@ -2956,14 +2916,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>$B$4="False"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="10">
+    <cfRule type="expression" dxfId="0" priority="10">
       <formula>$B$4="True"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:C13">
+  <conditionalFormatting sqref="B12:C12">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2973,7 +2933,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:C14">
+  <conditionalFormatting sqref="B13:C13">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="-1"/>
@@ -2983,7 +2943,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:C15">
+  <conditionalFormatting sqref="B14:C14">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2993,7 +2953,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:C16">
+  <conditionalFormatting sqref="B15:C15">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3003,7 +2963,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:C17">
+  <conditionalFormatting sqref="B16:C16">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3013,7 +2973,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:C18">
+  <conditionalFormatting sqref="B17:C17">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3023,7 +2983,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:C19">
+  <conditionalFormatting sqref="B18:C18">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3033,7 +2993,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20:C20">
+  <conditionalFormatting sqref="B19:C19">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="-1"/>

</xml_diff>

<commit_message>
io, #316, #322: Calculate formulas before saving.
</commit_message>
<xml_diff>
--- a/co2mpas/co2mpas_output_template.xlsx
+++ b/co2mpas/co2mpas_output_template.xlsx
@@ -1,16 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="37395" windowHeight="16755"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260"/>
   </bookViews>
   <sheets>
     <sheet name="output_report" sheetId="5" r:id="rId1"/>
     <sheet name="dice_report" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -287,7 +300,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,6 +376,12 @@
       <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -965,12 +984,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1000,12 +1019,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1215,22 +1234,22 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="0.42578125" style="5" hidden="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="5" hidden="1"/>
+    <col min="1" max="1" width="35.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0.5" style="5" hidden="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.95" customHeight="1">
+    <row r="1" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="2" t="str">
-        <f>IFERROR(IF([0]!_info_vehicle_family_id_Value&lt;&gt;"",[0]!_info_vehicle_family_id_Value,""), "")</f>
-        <v/>
+      <c r="B1" s="2" t="e">
+        <f ca="1">INDIRECT("summary!_info_vehicle_family_id_Value")</f>
+        <v>#REF!</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -1248,13 +1267,13 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="18.95" customHeight="1">
+    <row r="2" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="str">
-        <f>IFERROR(IF([0]!_info_CO2MPAS_version_Value&lt;&gt;"",[0]!_info_CO2MPAS_version_Value,""), "")</f>
-        <v/>
+      <c r="B2" s="2" t="e">
+        <f ca="1">INDIRECT("summary!_info_CO2MPAS_version_Value")</f>
+        <v>#REF!</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1272,13 +1291,13 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:17" ht="18.95" customHeight="1">
+    <row r="3" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="str">
-        <f>IFERROR(IF([0]!_info_Simulation_started_Value&lt;&gt;"",[0]!_info_Simulation_started_Value,""),"")</f>
-        <v/>
+      <c r="B3" s="2" t="e">
+        <f ca="1">INDIRECT("summary!_info_Simulation_started_Value")</f>
+        <v>#REF!</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1296,13 +1315,13 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:17" ht="18.95" customHeight="1">
+    <row r="4" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="str">
-        <f>IFERROR(IF([0]!_info_type_approval_mode_Value&lt;&gt;"",[0]!_info_type_approval_mode_Value,""),"")</f>
-        <v/>
+      <c r="B4" s="6" t="e">
+        <f ca="1">INDIRECT("summary!_info_type_approval_mode_Value")</f>
+        <v>#REF!</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="7"/>
@@ -1320,7 +1339,7 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:17" ht="18.95" customHeight="1">
+    <row r="5" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
@@ -1339,7 +1358,7 @@
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
     </row>
-    <row r="6" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
+    <row r="6" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
@@ -1358,7 +1377,7 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
     </row>
-    <row r="7" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
+    <row r="7" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>26</v>
       </c>
@@ -1385,17 +1404,17 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
     </row>
-    <row r="8" spans="1:17" ht="18.95" customHeight="1">
+    <row r="8" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="33" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_target_declared_co2_emission_declared_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_h_prediction_target_declared_co2_emission_declared_value__CO2g_km_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C8" s="34" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_l_prediction_target_declared_co2_emission_declared_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_l_prediction_target_declared_co2_emission_declared_value__CO2g_km_,""),"")</f>
-        <v/>
+      <c r="B8" s="33" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_target_declared_co2_emission_declared_value__CO2g_km_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C8" s="34" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_target_declared_co2_emission_declared_value__CO2g_km_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>28</v>
@@ -1414,17 +1433,17 @@
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
     </row>
-    <row r="9" spans="1:17" ht="18.95" customHeight="1">
+    <row r="9" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="35" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_declared_co2_emission_declared_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_declared_co2_emission_declared_value__CO2g_km_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C9" s="36" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_declared_co2_emission_declared_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_declared_co2_emission_declared_value__CO2g_km_,""),"")</f>
-        <v/>
+      <c r="B9" s="35" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_declared_co2_emission_declared_value__CO2g_km_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C9" s="36" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_declared_co2_emission_declared_value__CO2g_km_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>28</v>
@@ -1443,17 +1462,17 @@
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
     </row>
-    <row r="10" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
+    <row r="10" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="37" t="str">
-        <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio-1)*100,""),"")</f>
-        <v/>
-      </c>
-      <c r="C10" s="38" t="str">
-        <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio-1)*100,""),"")</f>
-        <v/>
+      <c r="B10" s="37" t="e">
+        <f ca="1">(INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio")-1)*100</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C10" s="38" t="e">
+        <f ca="1">(INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio")-1)*100</f>
+        <v>#REF!</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>25</v>
@@ -1472,7 +1491,7 @@
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
     </row>
-    <row r="11" spans="1:17" ht="18.95" customHeight="1">
+    <row r="11" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="39" t="s">
         <v>30</v>
       </c>
@@ -1493,7 +1512,7 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
     </row>
-    <row r="12" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
+    <row r="12" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="42"/>
       <c r="C12" s="3"/>
@@ -1512,7 +1531,7 @@
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
     </row>
-    <row r="13" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
+    <row r="13" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>31</v>
       </c>
@@ -1537,17 +1556,17 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
     </row>
-    <row r="14" spans="1:17" ht="18.95" customHeight="1">
+    <row r="14" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="44" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_co2_emission_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_co2_emission_value__CO2g_km_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C14" s="45" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_co2_emission_value__CO2g_km_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_co2_emission_value__CO2g_km_,""),"")</f>
-        <v/>
+      <c r="B14" s="44" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_value__CO2g_km_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C14" s="45" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_value__CO2g_km_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>28</v>
@@ -1566,17 +1585,17 @@
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
     </row>
-    <row r="15" spans="1:17" ht="18.95" customHeight="1">
+    <row r="15" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="35" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_co2_emission_UDC__CO2g_km_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_co2_emission_UDC__CO2g_km_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C15" s="36" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_co2_emission_UDC__CO2g_km_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_co2_emission_UDC__CO2g_km_,""),"")</f>
-        <v/>
+      <c r="B15" s="35" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_UDC__CO2g_km_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C15" s="36" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_UDC__CO2g_km_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>28</v>
@@ -1595,17 +1614,17 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="1:17" ht="18.95" customHeight="1" thickBot="1">
+    <row r="16" spans="1:17" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="46" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_co2_emission_EUDC__CO2g_km_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_co2_emission_EUDC__CO2g_km_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C16" s="47" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_co2_emission_EUDC__CO2g_km_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_co2_emission_EUDC__CO2g_km_,""),"")</f>
-        <v/>
+      <c r="B16" s="46" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_EUDC__CO2g_km_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C16" s="47" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_EUDC__CO2g_km_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>28</v>
@@ -1624,7 +1643,7 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
     </row>
-    <row r="17" spans="1:17" ht="18.95" customHeight="1">
+    <row r="17" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="42"/>
       <c r="C17" s="3"/>
@@ -1643,7 +1662,7 @@
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
     </row>
-    <row r="18" spans="1:17" ht="18.95" customHeight="1">
+    <row r="18" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="42"/>
       <c r="C18" s="3"/>
@@ -1662,7 +1681,7 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="1:17" ht="18.95" customHeight="1">
+    <row r="19" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="48" t="s">
         <v>35</v>
       </c>
@@ -1687,17 +1706,17 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="1:17" ht="18.95" customHeight="1">
+    <row r="20" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="35" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_f0__N_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_f0__N_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C20" s="35" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_f0__N_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_f0__N_,""),"")</f>
-        <v/>
+      <c r="B20" s="35" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f0__N_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C20" s="35" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f0__N_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>37</v>
@@ -1716,17 +1735,17 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="1:17" ht="18.95" customHeight="1">
+    <row r="21" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="51" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__,""),"")</f>
-        <v/>
-      </c>
-      <c r="C21" s="51" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__,""),"")</f>
-        <v/>
+      <c r="B21" s="51" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C21" s="51" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__")</f>
+        <v>#REF!</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>39</v>
@@ -1745,17 +1764,17 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
     </row>
-    <row r="22" spans="1:17" ht="18.95" customHeight="1">
+    <row r="22" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="51" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C22" s="51" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_,""),"")</f>
-        <v/>
+      <c r="B22" s="51" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C22" s="51" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>41</v>
@@ -1774,17 +1793,17 @@
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
     </row>
-    <row r="23" spans="1:17" ht="18.95" customHeight="1">
+    <row r="23" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="52" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_mass__kg_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_mass__kg_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C23" s="52" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_mass__kg_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_mass__kg_,""),"")</f>
-        <v/>
+      <c r="B23" s="52" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_mass__kg_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C23" s="52" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_mass__kg_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D23" s="53" t="s">
         <v>43</v>
@@ -1803,7 +1822,7 @@
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
     </row>
-    <row r="24" spans="1:17" ht="18.95" customHeight="1">
+    <row r="24" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="48" t="s">
         <v>44</v>
       </c>
@@ -1828,17 +1847,17 @@
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
     </row>
-    <row r="25" spans="1:17" ht="18.95" customHeight="1">
+    <row r="25" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="35" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_vehicle_f0__N_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_vehicle_f0__N_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C25" s="35" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_vehicle_f0__N_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_vehicle_f0__N_,""),"")</f>
-        <v/>
+      <c r="B25" s="35" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f0__N_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C25" s="35" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f0__N_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>37</v>
@@ -1857,17 +1876,17 @@
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
     </row>
-    <row r="26" spans="1:17" ht="18.95" customHeight="1">
+    <row r="26" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="51" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__&lt;&gt;"",[0]!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__,""),"")</f>
-        <v/>
-      </c>
-      <c r="C26" s="51" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__&lt;&gt;"",[0]!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__,""),"")</f>
-        <v/>
+      <c r="B26" s="51" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C26" s="51" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__")</f>
+        <v>#REF!</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>39</v>
@@ -1886,17 +1905,17 @@
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
     </row>
-    <row r="27" spans="1:17" ht="18.95" customHeight="1">
+    <row r="27" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="51" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C27" s="51" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_,""),"")</f>
-        <v/>
+      <c r="B27" s="51" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C27" s="51" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>41</v>
@@ -1915,17 +1934,17 @@
       <c r="P27" s="7"/>
       <c r="Q27" s="7"/>
     </row>
-    <row r="28" spans="1:17" ht="18.95" customHeight="1">
+    <row r="28" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="52" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_vehicle_mass__kg_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_vehicle_mass__kg_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C28" s="52" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_vehicle_mass__kg_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_vehicle_mass__kg_,""),"")</f>
-        <v/>
+      <c r="B28" s="52" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_mass__kg_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C28" s="52" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_mass__kg_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D28" s="53" t="s">
         <v>43</v>
@@ -1944,17 +1963,17 @@
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
     </row>
-    <row r="29" spans="1:17" ht="18.95" customHeight="1">
+    <row r="29" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="35" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C29" s="35" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_,""),"")</f>
-        <v/>
+      <c r="B29" s="35" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C29" s="35" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D29" s="53" t="s">
         <v>28</v>
@@ -1973,17 +1992,17 @@
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
     </row>
-    <row r="30" spans="1:17" ht="18.95" customHeight="1">
+    <row r="30" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="35" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C30" s="35" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_,""),"")</f>
-        <v/>
+      <c r="B30" s="35" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C30" s="35" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D30" s="53" t="s">
         <v>28</v>
@@ -2002,17 +2021,17 @@
       <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
     </row>
-    <row r="31" spans="1:17" ht="18.95" customHeight="1">
+    <row r="31" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="35" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_,""), "")</f>
-        <v/>
-      </c>
-      <c r="C31" s="35" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_,""),"")</f>
-        <v/>
+      <c r="B31" s="35" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C31" s="35" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D31" s="53" t="s">
         <v>28</v>
@@ -2031,17 +2050,17 @@
       <c r="P31" s="7"/>
       <c r="Q31" s="7"/>
     </row>
-    <row r="32" spans="1:17" ht="18.95" customHeight="1">
+    <row r="32" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="35" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_&lt;&gt;"",[0]!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C32" s="35" t="str">
-        <f>IFERROR(IF([0]!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_&lt;&gt;"",[0]!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_,""),"")</f>
-        <v/>
+      <c r="B32" s="35" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C32" s="35" t="e">
+        <f ca="1">INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D32" s="53" t="s">
         <v>28</v>
@@ -2060,7 +2079,7 @@
       <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
     </row>
-    <row r="33" spans="1:17" hidden="1">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2079,7 +2098,7 @@
       <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
     </row>
-    <row r="34" spans="1:17" hidden="1">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2098,7 +2117,7 @@
       <c r="P34" s="7"/>
       <c r="Q34" s="7"/>
     </row>
-    <row r="35" spans="1:17" hidden="1">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -2117,7 +2136,7 @@
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
     </row>
-    <row r="36" spans="1:17" hidden="1">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -2136,7 +2155,7 @@
       <c r="P36" s="7"/>
       <c r="Q36" s="7"/>
     </row>
-    <row r="37" spans="1:17" hidden="1">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -2155,7 +2174,7 @@
       <c r="P37" s="7"/>
       <c r="Q37" s="7"/>
     </row>
-    <row r="38" spans="1:17" hidden="1">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -2174,7 +2193,7 @@
       <c r="P38" s="7"/>
       <c r="Q38" s="7"/>
     </row>
-    <row r="39" spans="1:17" hidden="1">
+    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -2193,7 +2212,7 @@
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
     </row>
-    <row r="40" spans="1:17" hidden="1">
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -2212,7 +2231,7 @@
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
     </row>
-    <row r="41" spans="1:17" hidden="1">
+    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -2231,7 +2250,7 @@
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
     </row>
-    <row r="42" spans="1:17" hidden="1">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -2250,7 +2269,7 @@
       <c r="P42" s="7"/>
       <c r="Q42" s="7"/>
     </row>
-    <row r="43" spans="1:17" hidden="1">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -2270,6 +2289,8 @@
       <c r="Q43" s="7"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="B10:C10">
     <cfRule type="colorScale" priority="3">
       <colorScale>
@@ -2295,6 +2316,11 @@
   <headerFooter>
     <oddHeader>&amp;CCO2MPAS SUMMARY OUTPUT REPORT</oddHeader>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2306,22 +2332,22 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" style="28" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="28" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="0.42578125" style="28" hidden="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="28" hidden="1"/>
+    <col min="1" max="1" width="37.5" style="28" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0.5" style="28" hidden="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="28" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="2" t="str">
-        <f>IFERROR(IF([0]!_info_vehicle_family_id_Value&lt;&gt;"",[0]!_info_vehicle_family_id_Value,""), "")</f>
-        <v/>
+      <c r="B1" s="2" t="e">
+        <f ca="1">INDIRECT("summary!_info_vehicle_family_id_Value")</f>
+        <v>#REF!</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -2339,13 +2365,13 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="str">
-        <f>IFERROR(IF([0]!_info_CO2MPAS_version_Value&lt;&gt;"",[0]!_info_CO2MPAS_version_Value,""), "")</f>
-        <v/>
+      <c r="B2" s="2" t="e">
+        <f ca="1">INDIRECT("summary!_info_CO2MPAS_version_Value")</f>
+        <v>#REF!</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2363,13 +2389,13 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+    <row r="3" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="str">
-        <f>IFERROR(IF([0]!_info_Simulation_started_Value&lt;&gt;"",[0]!_info_Simulation_started_Value,""),"")</f>
-        <v/>
+      <c r="B3" s="2" t="e">
+        <f ca="1">INDIRECT("summary!_info_Simulation_started_Value")</f>
+        <v>#REF!</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2387,13 +2413,13 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+    <row r="4" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="str">
-        <f>IFERROR(IF([0]!_info_type_approval_mode_Value&lt;&gt;"",[0]!_info_type_approval_mode_Value,""),"")</f>
-        <v/>
+      <c r="B4" s="6" t="e">
+        <f ca="1">INDIRECT("summary!_info_type_approval_mode_Value")</f>
+        <v>#REF!</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="7"/>
@@ -2411,7 +2437,7 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+    <row r="5" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
@@ -2430,7 +2456,7 @@
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
     </row>
-    <row r="6" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
+    <row r="6" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
@@ -2449,7 +2475,7 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
     </row>
-    <row r="7" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
+    <row r="7" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
         <v>3</v>
@@ -2474,17 +2500,17 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
     </row>
-    <row r="8" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+    <row r="8" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_fuel_type__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_fuel_type__,""),"")</f>
-        <v/>
-      </c>
-      <c r="C8" s="14" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_fuel_type__&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_fuel_type__,""),"")</f>
-        <v/>
+      <c r="B8" s="13" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_fuel_type__")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C8" s="14" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_fuel_type__")</f>
+        <v>#REF!</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>7</v>
@@ -2503,17 +2529,17 @@
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
     </row>
-    <row r="9" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+    <row r="9" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_,""),"")</f>
-        <v/>
-      </c>
-      <c r="C9" s="17" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_,""),"")</f>
-        <v/>
+      <c r="B9" s="16" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C9" s="17" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_")</f>
+        <v>#REF!</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>9</v>
@@ -2532,17 +2558,17 @@
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
     </row>
-    <row r="10" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+    <row r="10" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="16" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_gear_box_type__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_gear_box_type__,""),"")</f>
-        <v/>
-      </c>
-      <c r="C10" s="17" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_gear_box_type__&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_gear_box_type__,""),"")</f>
-        <v/>
+      <c r="B10" s="16" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C10" s="17" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_gear_box_type__")</f>
+        <v>#REF!</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>7</v>
@@ -2561,17 +2587,17 @@
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
     </row>
-    <row r="11" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
+    <row r="11" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="19" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__&lt;&gt;"",[0]!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__,""),"")</f>
-        <v/>
-      </c>
-      <c r="C11" s="20" t="str">
-        <f>IFERROR(IF([0]!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__&lt;&gt;"",[0]!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__,""),"")</f>
-        <v/>
+      <c r="B11" s="19" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C11" s="20" t="e">
+        <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__")</f>
+        <v>#REF!</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>7</v>
@@ -2590,17 +2616,17 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
     </row>
-    <row r="12" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+    <row r="12" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="21" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_alternator_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_alternator_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C12" s="22" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_alternator_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_alternator_model_wltp_l_score,""),"")</f>
-        <v/>
+      <c r="B12" s="21" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_alternator_model_wltp_h_score")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C12" s="22" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_alternator_model_wltp_l_score")</f>
+        <v>#REF!</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>13</v>
@@ -2619,17 +2645,17 @@
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
     </row>
-    <row r="13" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+    <row r="13" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="21" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_at_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_at_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C13" s="22" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_at_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_at_model_wltp_l_score,""),"")</f>
-        <v/>
+      <c r="B13" s="21" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_at_model_wltp_h_score")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C13" s="22" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_at_model_wltp_l_score")</f>
+        <v>#REF!</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>7</v>
@@ -2648,17 +2674,17 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
     </row>
-    <row r="14" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+    <row r="14" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="21" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_clutch_torque_converter_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_clutch_torque_converter_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C14" s="22" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_clutch_torque_converter_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_clutch_torque_converter_model_wltp_l_score,""),"")</f>
-        <v/>
+      <c r="B14" s="21" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_clutch_torque_converter_model_wltp_h_score")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C14" s="22" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_clutch_torque_converter_model_wltp_l_score")</f>
+        <v>#REF!</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>16</v>
@@ -2677,17 +2703,17 @@
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
     </row>
-    <row r="15" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+    <row r="15" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="21" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_co2_params_wltp_h_score&lt;&gt;"",[0]!_score_by_model_co2_params_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C15" s="22" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_co2_params_wltp_l_score&lt;&gt;"",[0]!_score_by_model_co2_params_wltp_l_score,""),"")</f>
-        <v/>
+      <c r="B15" s="21" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_co2_params_wltp_h_score")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C15" s="22" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_co2_params_wltp_l_score")</f>
+        <v>#REF!</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>18</v>
@@ -2706,17 +2732,17 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+    <row r="16" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="21" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_cold_start_speed_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_cold_start_speed_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C16" s="22" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_cold_start_speed_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_cold_start_speed_model_wltp_l_score,""),"")</f>
-        <v/>
+      <c r="B16" s="21" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_cold_start_speed_model_wltp_h_score")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C16" s="22" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_cold_start_speed_model_wltp_l_score")</f>
+        <v>#REF!</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>16</v>
@@ -2735,17 +2761,17 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
     </row>
-    <row r="17" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+    <row r="17" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="21" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_coolant_temperature_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_coolant_temperature_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C17" s="22" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_coolant_temperature_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_coolant_temperature_model_wltp_l_score,""),"")</f>
-        <v/>
+      <c r="B17" s="21" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_coolant_temperature_model_wltp_h_score")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C17" s="22" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_coolant_temperature_model_wltp_l_score")</f>
+        <v>#REF!</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>21</v>
@@ -2764,17 +2790,17 @@
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
     </row>
-    <row r="18" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1">
+    <row r="18" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="21" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_speed_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_engine_speed_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C18" s="22" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_engine_speed_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_engine_speed_model_wltp_l_score,""),"")</f>
-        <v/>
+      <c r="B18" s="21" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_speed_model_wltp_h_score")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C18" s="22" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_speed_model_wltp_l_score")</f>
+        <v>#REF!</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>16</v>
@@ -2793,17 +2819,17 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
+    <row r="19" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="23" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_start_stop_model_wltp_h_score&lt;&gt;"",[0]!_score_by_model_start_stop_model_wltp_h_score,""),"")</f>
-        <v/>
-      </c>
-      <c r="C19" s="24" t="str">
-        <f>IFERROR(IF([0]!_score_by_model_start_stop_model_wltp_l_score&lt;&gt;"",[0]!_score_by_model_start_stop_model_wltp_l_score,""),"")</f>
-        <v/>
+      <c r="B19" s="23" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_start_stop_model_wltp_h_score")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C19" s="24" t="e">
+        <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_start_stop_model_wltp_l_score")</f>
+        <v>#REF!</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>7</v>
@@ -2822,17 +2848,17 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="1:17" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
+    <row r="20" spans="1:17" s="5" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="26" t="str">
-        <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio-1)*100,""),"")</f>
-        <v/>
-      </c>
-      <c r="C20" s="27" t="str">
-        <f>IFERROR(IF([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio&lt;&gt;"",([0]!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio-1)*100,""),"")</f>
-        <v/>
+      <c r="B20" s="26" t="e">
+        <f ca="1">(INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio")-1)*100</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C20" s="27" t="e">
+        <f ca="1">(INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio")-1)*100</f>
+        <v>#REF!</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>25</v>
@@ -2851,7 +2877,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="1:17" s="5" customFormat="1" ht="18.95" hidden="1" customHeight="1">
+    <row r="21" spans="1:17" s="5" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -2866,43 +2892,44 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
     </row>
-    <row r="22" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="23" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="24" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="25" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="26" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="27" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="28" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="29" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="30" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="31" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="32" spans="1:17" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="33" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="34" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="35" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="36" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="37" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="38" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="39" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="40" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="41" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="42" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="43" ht="18.95" hidden="1" customHeight="1"/>
-    <row r="44" ht="15" hidden="1" customHeight="1"/>
-    <row r="45" ht="15" hidden="1" customHeight="1"/>
-    <row r="46" ht="15" hidden="1" customHeight="1"/>
-    <row r="47" ht="15" hidden="1" customHeight="1"/>
-    <row r="48" ht="15" hidden="1" customHeight="1"/>
-    <row r="49" ht="15" hidden="1" customHeight="1"/>
-    <row r="50" ht="15" hidden="1" customHeight="1"/>
-    <row r="51" ht="15" hidden="1" customHeight="1"/>
-    <row r="52" ht="15" hidden="1" customHeight="1"/>
-    <row r="53" ht="15" hidden="1" customHeight="1"/>
-    <row r="54" ht="15" hidden="1" customHeight="1"/>
-    <row r="55" ht="15" hidden="1" customHeight="1"/>
-    <row r="56" ht="15" hidden="1" customHeight="1"/>
+    <row r="22" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:17" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="B20:C20">
     <cfRule type="colorScale" priority="11">
       <colorScale>
@@ -3008,5 +3035,10 @@
   <headerFooter>
     <oddHeader>&amp;CCO2MPAS DICE REPORT</oddHeader>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>